<commit_message>
cargado de datos terminado
</commit_message>
<xml_diff>
--- a/Saves/aa.xlsx
+++ b/Saves/aa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Sheet"/>
@@ -56,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +67,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -106,10 +112,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -419,7 +425,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -669,7 +675,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>